<commit_message>
temp files to aid in transfer to gsheets
</commit_message>
<xml_diff>
--- a/saved_versions/alltemp_codejoins.xlsx
+++ b/saved_versions/alltemp_codejoins.xlsx
@@ -527,7 +527,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html' target='_blank'&gt;https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
@@ -746,7 +746,7 @@
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html' target='_blank'&gt;https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q5">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="O18" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html' target='_blank'&gt;https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="P18" t="inlineStr">
@@ -2172,7 +2172,7 @@
       </c>
       <c r="O24" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html' target='_blank'&gt;https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="P24" t="inlineStr">
@@ -5360,7 +5360,7 @@
       </c>
       <c r="O63" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html' target='_blank'&gt;https://www.cnn.com/2019/08/21/politics/fact-check-trump-84-false-claims-last-week/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="P63" t="inlineStr">
@@ -8231,7 +8231,7 @@
       </c>
       <c r="O100" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/08/14/politics/weekly-fact-check-donald-trump-21-false/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/08/14/politics/weekly-fact-check-donald-trump-21-false/index.html' target='_blank'&gt;https://www.cnn.com/2019/08/14/politics/weekly-fact-check-donald-trump-21-false/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="P100" t="inlineStr">
@@ -8319,7 +8319,7 @@
       </c>
       <c r="O101" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/08/07/politics/fact-check-trump-brown-hospital-visit-dayton/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/08/07/politics/fact-check-trump-brown-hospital-visit-dayton/index.html' target='_blank'&gt;https://www.cnn.com/2019/08/07/politics/fact-check-trump-brown-hospital-visit-dayton/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="P101" t="inlineStr">
@@ -19903,7 +19903,7 @@
       </c>
       <c r="O248" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/23/politics/weekly-trump-fact-check-july-2019-61-false/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/23/politics/weekly-trump-fact-check-july-2019-61-false/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/23/politics/weekly-trump-fact-check-july-2019-61-false/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q248">
@@ -20701,7 +20701,7 @@
       </c>
       <c r="O258" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q258">
@@ -20792,7 +20792,7 @@
       </c>
       <c r="O259" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q259">
@@ -20882,7 +20882,7 @@
       </c>
       <c r="O260" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q260">
@@ -20974,7 +20974,7 @@
       </c>
       <c r="O261" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q261">
@@ -21071,7 +21071,7 @@
       </c>
       <c r="O262" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q262">
@@ -21159,7 +21159,7 @@
       </c>
       <c r="O263" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q263">
@@ -21252,7 +21252,7 @@
       </c>
       <c r="O264" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q264">
@@ -21340,7 +21340,7 @@
       </c>
       <c r="O265" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q265">
@@ -21432,7 +21432,7 @@
       </c>
       <c r="O266" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q266">
@@ -21519,7 +21519,7 @@
       </c>
       <c r="O267" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q267">
@@ -21611,7 +21611,7 @@
       </c>
       <c r="O268" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q268">
@@ -21697,7 +21697,7 @@
       </c>
       <c r="O269" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q269">
@@ -21795,7 +21795,7 @@
       </c>
       <c r="O270" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q270">
@@ -21887,7 +21887,7 @@
       </c>
       <c r="O271" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q271">
@@ -21978,7 +21978,7 @@
       </c>
       <c r="O272" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q272">
@@ -22074,7 +22074,7 @@
       </c>
       <c r="O273" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q273">
@@ -22165,7 +22165,7 @@
       </c>
       <c r="O274" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q274">
@@ -22258,7 +22258,7 @@
       </c>
       <c r="O275" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q275">
@@ -22339,7 +22339,7 @@
       </c>
       <c r="O276" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q276">
@@ -22761,7 +22761,7 @@
       </c>
       <c r="O281" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q281">
@@ -22842,7 +22842,7 @@
       </c>
       <c r="O282" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q282">
@@ -22930,7 +22930,7 @@
       </c>
       <c r="O283" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q283">
@@ -23011,7 +23011,7 @@
       </c>
       <c r="O284" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q284">
@@ -23088,7 +23088,7 @@
       </c>
       <c r="O285" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q285">
@@ -23175,7 +23175,7 @@
       </c>
       <c r="O286" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q286">
@@ -23261,7 +23261,7 @@
       </c>
       <c r="O287" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q287">
@@ -23343,7 +23343,7 @@
       </c>
       <c r="O288" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q288">
@@ -23429,7 +23429,7 @@
       </c>
       <c r="O289" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q289">
@@ -23520,7 +23520,7 @@
       </c>
       <c r="O290" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q290">
@@ -23611,7 +23611,7 @@
       </c>
       <c r="O291" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q291">
@@ -23692,7 +23692,7 @@
       </c>
       <c r="O292" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q292">
@@ -23781,7 +23781,7 @@
       </c>
       <c r="O293" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/16/politics/donald-trump-fact-check-cabinet-meeting/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q293">
@@ -24032,7 +24032,7 @@
       </c>
       <c r="O296" t="inlineStr">
         <is>
-          <t>https://www.whitehouse.gov/briefings-statements/remarks-president-trump-marine-one-departure-53/</t>
+          <t>&lt;a href='https://www.whitehouse.gov/briefings-statements/remarks-president-trump-marine-one-departure-53/' target='_blank'&gt;https://www.whitehouse.gov/briefings-statements/remarks-president-trump-marine-one-departure-53/&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q296">
@@ -24420,7 +24420,7 @@
       </c>
       <c r="O301" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/23/politics/trump-fact-check-week-july-8-to-july-14/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/23/politics/trump-fact-check-week-july-8-to-july-14/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/23/politics/trump-fact-check-week-july-8-to-july-14/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q301">
@@ -26999,7 +26999,7 @@
       </c>
       <c r="O334" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/08/21/politics/fact-check-trump-11-false-claims-greenland/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/08/21/politics/fact-check-trump-11-false-claims-greenland/index.html' target='_blank'&gt;https://www.cnn.com/2019/08/21/politics/fact-check-trump-11-false-claims-greenland/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="P334" t="inlineStr">
@@ -27599,7 +27599,7 @@
       </c>
       <c r="O342" t="inlineStr">
         <is>
-          <t>https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html</t>
+          <t>&lt;a href='https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html' target='_blank'&gt;https://www.cnn.com/2019/07/18/politics/trump-false-claims-in-greenville-north-carolina-rally/index.html&lt;/a&gt;</t>
         </is>
       </c>
       <c r="Q342">

</xml_diff>